<commit_message>
Added sockets for IMU, Sensors and ODrives
</commit_message>
<xml_diff>
--- a/schematics/CentralBoard/bom.xlsx
+++ b/schematics/CentralBoard/bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Lisbeth\schematics\CentralBoard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3FAFEA9-FFD3-48C1-8428-B869245AAB9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E34C43FF-7F30-49BB-9A94-F8F1FA987068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6615" yWindow="9000" windowWidth="38700" windowHeight="15375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="15" windowWidth="28770" windowHeight="16170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>https://eu.mouser.com/ProductDetail/Diodes-Incorporated/DMTH8003SPS-13?qs=fAHHVMwC%252BbjFPwZ285SuFQ%3D%3D</t>
   </si>
@@ -42,9 +42,6 @@
     <t>U2</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>MOSFET 100V, 100A</t>
   </si>
   <si>
@@ -69,9 +66,6 @@
     <t>U1</t>
   </si>
   <si>
-    <t>https://www.digikey.de/en/products/detail/analog-devices-inc/LTC4440ES6-TRMPBF/1116021</t>
-  </si>
-  <si>
     <t>Mouser</t>
   </si>
   <si>
@@ -88,6 +82,45 @@
   </si>
   <si>
     <t>IC2</t>
+  </si>
+  <si>
+    <t>Shunt 0.0004Ohm</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/de/products/detail/analog-devices-inc/LTC7001IMSE-PBF/7363804?utm_medium=email&amp;utm_source=oce&amp;utm_campaign=3310_OCE22RT&amp;utm_content=productdetail_DE&amp;utm_cid=2355993&amp;so=75928733&amp;mkt_tok=MDI4LVNYSy01MDcAAAGEemh6Hpx5pIinyDJpdIZawselVf67jNKToa_lz8TVHDCvkXFgNdSQy3jIBmqhnW0PfZFyGL8vHVQNrkMXCLy7Lbft8ti-Gt_-2fDYM6qN</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/de/products/detail/stmicroelectronics/STL100N10F7/3993110?utm_medium=email&amp;utm_source=oce&amp;utm_campaign=3310_OCE22RT&amp;utm_content=productdetail_DE&amp;utm_cid=2355993&amp;so=75928733&amp;mkt_tok=MDI4LVNYSy01MDcAAAGEemh6HtzLz_P-FEsSsUaBfWxGdHeMKJiNMf369mj9_Qi4I8NoYL4rC2tRRaQ6gPFC7QiGalt27_JUSQXtyGJ6SEnBeNibavWHfdGxt7tI</t>
+  </si>
+  <si>
+    <t>ordered</t>
+  </si>
+  <si>
+    <t>stock</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/de/products/detail/analog-devices-inc-maxim-integrated/MAX3222ECWN-T/1514556?utm_medium=email&amp;utm_source=oce&amp;utm_campaign=3310_OCE22RT&amp;utm_content=productdetail_DE&amp;utm_cid=2355993&amp;so=75928733&amp;mkt_tok=MDI4LVNYSy01MDcAAAGEemh6Hn6FuIg2MPNw_UjWh-MqLqpeDh-4ApnQN1rfi1xcU3gAKpXXwtZ6H_xmgn_GxLTfSQwX3hPh8praGgpQrDjMwOVEJ7bu-RNTSunv</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/de/products/detail/diodes-incorporated/AP2128K-3-3TRG1/4470794?utm_medium=email&amp;utm_source=oce&amp;utm_campaign=3310_OCE22RT&amp;utm_content=productdetail_DE&amp;utm_cid=2355993&amp;so=75928733&amp;mkt_tok=MDI4LVNYSy01MDcAAAGEemh6HiH8Ix77lNwS2cJN_lzQKPKLqLrsaAkrIbvSELvLyJU9B5mfv1IBClFA5cLAUc3v88LjuVqWKmKZjzP_SV1NQiHZT8n-iJQGX9HF</t>
+  </si>
+  <si>
+    <t>LDO Regulator 3.3.V</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>AP2128K-3.3TRG1</t>
   </si>
 </sst>
 </file>
@@ -409,21 +442,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="114.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="114.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -431,22 +465,31 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="F1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>16</v>
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -457,59 +500,118 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
         <v>0</v>
       </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>9</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3">
+        <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
         <v>20</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>